<commit_message>
Finished and working sol_laplace_equation_axb.m
</commit_message>
<xml_diff>
--- a/provaM2project1.xlsx
+++ b/provaM2project1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergi/FacturaDataset/13/annot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JosepM\Desktop\MasterCV\project\Optimisation-and-Inference-for-Computer-Vision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8CD0F0A-209C-4642-B585-683D1E01E65B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BDE7FF6A-C940-894A-81D9-2A3DBBD19BCF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="144">
   <si>
     <t>v11</t>
   </si>
@@ -410,13 +410,75 @@
   <si>
     <t>u36</t>
   </si>
+  <si>
+    <t>Mat original</t>
+  </si>
+  <si>
+    <t>mask inpaint</t>
+  </si>
+  <si>
+    <t>mat extended</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>b5</t>
+  </si>
+  <si>
+    <t>b7</t>
+  </si>
+  <si>
+    <t>b9</t>
+  </si>
+  <si>
+    <t>b10</t>
+  </si>
+  <si>
+    <t>b11</t>
+  </si>
+  <si>
+    <t>b12</t>
+  </si>
+  <si>
+    <t>b6</t>
+  </si>
+  <si>
+    <t>b8</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>mat a</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -444,8 +506,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,74 +822,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BA4264-BE70-384F-8994-755F0A3CB63E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="CA8" sqref="CA8"/>
+    <sheetView topLeftCell="Z1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="BZ1" sqref="BZ1:BZ8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="4.83203125" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" customWidth="1"/>
-    <col min="5" max="5" width="4.83203125" customWidth="1"/>
+    <col min="1" max="2" width="4.625" customWidth="1"/>
+    <col min="3" max="3" width="4.875" customWidth="1"/>
+    <col min="4" max="4" width="4.625" customWidth="1"/>
+    <col min="5" max="5" width="4.875" customWidth="1"/>
     <col min="6" max="6" width="4.5" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" customWidth="1"/>
-    <col min="8" max="8" width="4.83203125" customWidth="1"/>
+    <col min="7" max="7" width="4.625" customWidth="1"/>
+    <col min="8" max="8" width="4.875" customWidth="1"/>
     <col min="9" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="4.83203125" customWidth="1"/>
-    <col min="12" max="13" width="5.6640625" customWidth="1"/>
+    <col min="11" max="11" width="4.875" customWidth="1"/>
+    <col min="12" max="13" width="5.625" customWidth="1"/>
     <col min="14" max="14" width="4.5" customWidth="1"/>
-    <col min="15" max="15" width="5.33203125" customWidth="1"/>
+    <col min="15" max="15" width="5.375" customWidth="1"/>
     <col min="16" max="23" width="5" customWidth="1"/>
-    <col min="24" max="25" width="5.1640625" customWidth="1"/>
-    <col min="26" max="27" width="5.6640625" customWidth="1"/>
-    <col min="28" max="28" width="5.1640625" customWidth="1"/>
+    <col min="24" max="25" width="5.125" customWidth="1"/>
+    <col min="26" max="27" width="5.625" customWidth="1"/>
+    <col min="28" max="28" width="5.125" customWidth="1"/>
     <col min="29" max="29" width="5.5" customWidth="1"/>
-    <col min="30" max="30" width="5.33203125" customWidth="1"/>
-    <col min="31" max="31" width="5.6640625" customWidth="1"/>
-    <col min="32" max="32" width="5.1640625" customWidth="1"/>
-    <col min="33" max="34" width="4.83203125" customWidth="1"/>
-    <col min="35" max="35" width="5.33203125" customWidth="1"/>
-    <col min="36" max="36" width="5.1640625" customWidth="1"/>
-    <col min="37" max="37" width="5.33203125" customWidth="1"/>
-    <col min="38" max="38" width="4.33203125" customWidth="1"/>
+    <col min="30" max="30" width="5.375" customWidth="1"/>
+    <col min="31" max="31" width="5.625" customWidth="1"/>
+    <col min="32" max="32" width="5.125" customWidth="1"/>
+    <col min="33" max="34" width="4.875" customWidth="1"/>
+    <col min="35" max="35" width="5.375" customWidth="1"/>
+    <col min="36" max="36" width="5.125" customWidth="1"/>
+    <col min="37" max="37" width="5.375" customWidth="1"/>
+    <col min="38" max="38" width="4.375" customWidth="1"/>
     <col min="39" max="39" width="5" customWidth="1"/>
     <col min="40" max="41" width="5.5" customWidth="1"/>
-    <col min="42" max="44" width="5.33203125" customWidth="1"/>
-    <col min="45" max="45" width="5.6640625" customWidth="1"/>
-    <col min="46" max="46" width="5.83203125" customWidth="1"/>
+    <col min="42" max="44" width="5.375" customWidth="1"/>
+    <col min="45" max="45" width="5.625" customWidth="1"/>
+    <col min="46" max="46" width="5.875" customWidth="1"/>
     <col min="47" max="47" width="5" customWidth="1"/>
-    <col min="48" max="48" width="5.33203125" customWidth="1"/>
-    <col min="49" max="49" width="5.6640625" customWidth="1"/>
-    <col min="50" max="50" width="5.83203125" customWidth="1"/>
-    <col min="51" max="53" width="5.33203125" customWidth="1"/>
+    <col min="48" max="48" width="5.375" customWidth="1"/>
+    <col min="49" max="49" width="5.625" customWidth="1"/>
+    <col min="50" max="50" width="5.875" customWidth="1"/>
+    <col min="51" max="53" width="5.375" customWidth="1"/>
     <col min="54" max="54" width="5" customWidth="1"/>
     <col min="55" max="56" width="5.5" customWidth="1"/>
     <col min="57" max="57" width="5" customWidth="1"/>
     <col min="58" max="58" width="4.5" customWidth="1"/>
-    <col min="59" max="59" width="5.33203125" customWidth="1"/>
+    <col min="59" max="59" width="5.375" customWidth="1"/>
     <col min="60" max="60" width="6" customWidth="1"/>
-    <col min="61" max="61" width="5.1640625" customWidth="1"/>
-    <col min="62" max="62" width="5.83203125" customWidth="1"/>
+    <col min="61" max="61" width="5.125" customWidth="1"/>
+    <col min="62" max="62" width="5.875" customWidth="1"/>
     <col min="63" max="63" width="6" customWidth="1"/>
     <col min="64" max="64" width="5.5" customWidth="1"/>
     <col min="65" max="65" width="5" customWidth="1"/>
-    <col min="66" max="66" width="5.33203125" customWidth="1"/>
-    <col min="67" max="67" width="5.1640625" customWidth="1"/>
-    <col min="68" max="68" width="4.83203125" customWidth="1"/>
-    <col min="69" max="69" width="4.6640625" customWidth="1"/>
-    <col min="70" max="70" width="5.1640625" customWidth="1"/>
-    <col min="71" max="71" width="5.33203125" customWidth="1"/>
-    <col min="72" max="72" width="5.1640625" customWidth="1"/>
-    <col min="73" max="73" width="5.33203125" customWidth="1"/>
-    <col min="74" max="74" width="6.83203125" customWidth="1"/>
+    <col min="66" max="66" width="5.375" customWidth="1"/>
+    <col min="67" max="67" width="5.125" customWidth="1"/>
+    <col min="68" max="68" width="4.875" customWidth="1"/>
+    <col min="69" max="69" width="4.625" customWidth="1"/>
+    <col min="70" max="70" width="5.125" customWidth="1"/>
+    <col min="71" max="71" width="5.375" customWidth="1"/>
+    <col min="72" max="72" width="5.125" customWidth="1"/>
+    <col min="73" max="73" width="5.375" customWidth="1"/>
+    <col min="74" max="74" width="6.875" customWidth="1"/>
     <col min="75" max="75" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -1059,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1292,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1525,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1758,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1991,7 +2054,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2224,7 +2287,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2457,7 +2520,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2690,7 +2753,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -2923,7 +2986,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3156,7 +3219,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3389,7 +3452,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3622,7 +3685,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -3855,7 +3918,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4088,7 +4151,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -4321,7 +4384,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -4554,7 +4617,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -4787,7 +4850,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -5020,7 +5083,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -5253,7 +5316,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -5486,7 +5549,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -5719,7 +5782,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -5952,7 +6015,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -6185,7 +6248,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -6418,7 +6481,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -6651,7 +6714,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -6884,7 +6947,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -7117,7 +7180,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -7350,7 +7413,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -7583,7 +7646,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -7816,7 +7879,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -8049,7 +8112,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -8282,7 +8345,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0</v>
       </c>
@@ -8515,7 +8578,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -8748,7 +8811,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0</v>
       </c>
@@ -8981,7 +9044,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -9214,7 +9277,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0</v>
       </c>
@@ -9447,7 +9510,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0</v>
       </c>
@@ -9680,7 +9743,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0</v>
       </c>
@@ -9913,7 +9976,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -10146,7 +10209,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
@@ -10379,7 +10442,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -10612,7 +10675,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0</v>
       </c>
@@ -10845,7 +10908,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0</v>
       </c>
@@ -11078,7 +11141,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0</v>
       </c>
@@ -11311,7 +11374,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0</v>
       </c>
@@ -11544,7 +11607,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0</v>
       </c>
@@ -11777,7 +11840,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0</v>
       </c>
@@ -12010,7 +12073,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0</v>
       </c>
@@ -12243,7 +12306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0</v>
       </c>
@@ -12476,7 +12539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0</v>
       </c>
@@ -12709,7 +12772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0</v>
       </c>
@@ -12942,7 +13005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0</v>
       </c>
@@ -13175,7 +13238,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0</v>
       </c>
@@ -13408,7 +13471,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0</v>
       </c>
@@ -13641,7 +13704,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0</v>
       </c>
@@ -13874,7 +13937,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0</v>
       </c>
@@ -14107,7 +14170,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0</v>
       </c>
@@ -14340,7 +14403,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0</v>
       </c>
@@ -14573,7 +14636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>0</v>
       </c>
@@ -14806,7 +14869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0</v>
       </c>
@@ -15039,7 +15102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0</v>
       </c>
@@ -15272,7 +15335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0</v>
       </c>
@@ -15505,7 +15568,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0</v>
       </c>
@@ -15738,7 +15801,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0</v>
       </c>
@@ -15971,7 +16034,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="66" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0</v>
       </c>
@@ -16204,7 +16267,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-1</v>
       </c>
@@ -16437,7 +16500,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0</v>
       </c>
@@ -16670,7 +16733,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0</v>
       </c>
@@ -16903,7 +16966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0</v>
       </c>
@@ -17136,7 +17199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0</v>
       </c>
@@ -17369,7 +17432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0</v>
       </c>
@@ -17602,7 +17665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0</v>
       </c>
@@ -17835,7 +17898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0</v>
       </c>
@@ -18070,5 +18133,642 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>137</v>
+      </c>
+      <c r="J19" t="s">
+        <v>132</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19" t="s">
+        <v>138</v>
+      </c>
+      <c r="N19" t="s">
+        <v>133</v>
+      </c>
+      <c r="O19" t="s">
+        <v>140</v>
+      </c>
+      <c r="P19" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>-1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>-1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20" t="s">
+        <v>142</v>
+      </c>
+      <c r="T20" t="s">
+        <v>129</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="U21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="U22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>-1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>-1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>-1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>-1</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>-1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>-1</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="U27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="U28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>138</v>
+      </c>
+      <c r="U31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>133</v>
+      </c>
+      <c r="U32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>140</v>
+      </c>
+      <c r="U33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>141</v>
+      </c>
+      <c r="U34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>139</v>
+      </c>
+      <c r="U35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>